<commit_message>
RSEQREP v1.1.0 --  see release notes for updates
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VID\jgoll\projects\cloud-review-article\RSEQREP\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VID\tjensen\eclipse-projects\RSEQREP\RSEQREP\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -248,9 +248,6 @@
     <t>trtc</t>
   </si>
   <si>
-    <t>Output location to where pre-processing results will be written (directory must exist).</t>
-  </si>
-  <si>
     <t>The number of threads to be used for pre-processing.</t>
   </si>
   <si>
@@ -291,9 +288,6 @@
   </si>
   <si>
     <t>HISAT2 Aligner program location (if not used; leave it blank).</t>
-  </si>
-  <si>
-    <t>Output location to where the analysis files and report will be written (directory must exist).</t>
   </si>
   <si>
     <t>Long title to be used in the report (title page).</t>
@@ -708,6 +702,12 @@
       </rPr>
       <t xml:space="preserve"> Options: complete, single, average.</t>
     </r>
+  </si>
+  <si>
+    <t>Output location to where pre-processing results will be written.</t>
+  </si>
+  <si>
+    <t>Output location to where the analysis files and report will be written.</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1151,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1437,7 +1439,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1457,12 +1461,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="C2" s="6"/>
     </row>
@@ -1471,7 +1475,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="6"/>
     </row>
@@ -1480,7 +1484,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -1489,7 +1493,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -1498,7 +1502,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1507,7 +1511,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1516,7 +1520,7 @@
         <v>29</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -1525,7 +1529,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -1534,7 +1538,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="6"/>
     </row>
@@ -1543,7 +1547,7 @@
         <v>66</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="6"/>
     </row>
@@ -1552,7 +1556,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -1561,7 +1565,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="6"/>
     </row>
@@ -1570,7 +1574,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="6"/>
     </row>
@@ -1579,7 +1583,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="6"/>
     </row>
@@ -1588,7 +1592,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="6"/>
     </row>
@@ -1597,7 +1601,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="6"/>
     </row>
@@ -1606,7 +1610,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="6"/>
     </row>
@@ -1615,7 +1619,7 @@
         <v>65</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" s="6"/>
     </row>
@@ -1629,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection sqref="A1:B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1660,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="C2" s="6"/>
     </row>
@@ -1665,7 +1669,7 @@
         <v>64</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C3" s="6"/>
     </row>
@@ -1674,25 +1678,25 @@
         <v>63</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1701,7 +1705,7 @@
         <v>56</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1710,7 +1714,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -1719,16 +1723,16 @@
         <v>52</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C10" s="6"/>
     </row>
@@ -1737,16 +1741,16 @@
         <v>67</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -1755,7 +1759,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C13" s="6"/>
     </row>
@@ -1764,7 +1768,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C14" s="6"/>
     </row>
@@ -1773,25 +1777,25 @@
         <v>60</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C17" s="6"/>
     </row>
@@ -1800,7 +1804,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C18" s="6"/>
     </row>
@@ -1809,7 +1813,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C19" s="6"/>
     </row>
@@ -1818,7 +1822,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C20" s="6"/>
     </row>
@@ -1827,7 +1831,7 @@
         <v>59</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C21" s="6"/>
     </row>
@@ -1836,7 +1840,7 @@
         <v>30</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C22" s="6"/>
     </row>
@@ -1845,7 +1849,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C23" s="6"/>
     </row>
@@ -1854,7 +1858,7 @@
         <v>57</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C24" s="6"/>
     </row>
@@ -1863,7 +1867,7 @@
         <v>61</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C25" s="6"/>
     </row>
@@ -1872,7 +1876,7 @@
         <v>62</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" s="6"/>
     </row>
@@ -1881,7 +1885,7 @@
         <v>68</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C27" s="6"/>
     </row>

</xml_diff>